<commit_message>
Add sprint 2 user stories, and presentation
</commit_message>
<xml_diff>
--- a/docs/efforts/Luis Ramirez.xlsx
+++ b/docs/efforts/Luis Ramirez.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LouieBoy\Documents\GitHub\GPTMS\docs\efforts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A206CA2F-6D9B-4D70-966A-CB6250524F40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67740288-CD8C-4062-9D8D-AD4D281F38E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3870" yWindow="960" windowWidth="26385" windowHeight="11490" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="300" yWindow="1095" windowWidth="26385" windowHeight="11490" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Evidence" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t>Brief Description of Acomplishments</t>
   </si>
@@ -145,13 +145,16 @@
     <t xml:space="preserve">signup component
 Slides 3, 5-7
 </t>
+  </si>
+  <si>
+    <t>1, 2, 3, 5, 6[CS,IT]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -195,6 +198,14 @@
       <b/>
       <sz val="20"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -299,8 +310,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -338,11 +350,23 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -364,18 +388,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -388,9 +400,10 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -671,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -688,38 +701,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
     </row>
     <row r="2" spans="1:8" ht="41.1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="17" t="s">
+      <c r="B2" s="23"/>
+      <c r="C2" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="25"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="18"/>
     </row>
     <row r="3" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="21"/>
+      <c r="B3" s="25"/>
       <c r="C3" s="4" t="s">
         <v>7</v>
       </c>
@@ -740,10 +753,10 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="114.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="22"/>
+      <c r="B4" s="26"/>
       <c r="C4" s="11">
         <v>16</v>
       </c>
@@ -763,15 +776,17 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+    <row r="5" spans="1:8" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="15">
+      <c r="B5" s="26"/>
+      <c r="C5" s="14">
         <v>16</v>
       </c>
-      <c r="D5" s="14"/>
+      <c r="D5" s="15" t="s">
+        <v>36</v>
+      </c>
       <c r="E5" s="12" t="s">
         <v>34</v>
       </c>
@@ -784,10 +799,10 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="16"/>
+      <c r="B6" s="20"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="2"/>
@@ -796,10 +811,10 @@
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="16"/>
+      <c r="B7" s="20"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="2"/>
@@ -808,10 +823,10 @@
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="16"/>
+      <c r="B8" s="20"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="2"/>
@@ -820,10 +835,10 @@
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="16"/>
+      <c r="B9" s="20"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="2"/>
@@ -832,10 +847,10 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="16"/>
+      <c r="B10" s="20"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="2"/>
@@ -844,10 +859,10 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="16"/>
+      <c r="B11" s="20"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="2"/>
@@ -856,10 +871,10 @@
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="16"/>
+      <c r="B12" s="20"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="2"/>
@@ -868,10 +883,10 @@
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="16"/>
+      <c r="B13" s="20"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="2"/>
@@ -880,10 +895,10 @@
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="16"/>
+      <c r="B14" s="20"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="2"/>
@@ -892,10 +907,10 @@
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="16"/>
+      <c r="B15" s="20"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="2"/>
@@ -905,11 +920,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="A2:B2"/>
@@ -923,6 +933,11 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -934,7 +949,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -962,19 +977,19 @@
       <c r="I1" s="29"/>
     </row>
     <row r="2" spans="1:9" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="17" t="s">
+      <c r="B2" s="23"/>
+      <c r="C2" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="19"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="23"/>
     </row>
     <row r="3" spans="1:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27"/>
@@ -1096,13 +1111,13 @@
         <v>0</v>
       </c>
       <c r="G7" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H7" s="8">
         <v>3</v>
       </c>
       <c r="I7" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update effort logbook for Sprint3
</commit_message>
<xml_diff>
--- a/docs/efforts/Luis Ramirez.xlsx
+++ b/docs/efforts/Luis Ramirez.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LouieBoy\Documents\GitHub\GPTMS\docs\efforts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48AF8728-0DA7-4988-A83D-7A84869DF118}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18F1920B-954C-4518-B65F-12AF62E3E5DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2175" yWindow="1395" windowWidth="26385" windowHeight="11490" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11835" yWindow="1815" windowWidth="16935" windowHeight="11490" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Evidence" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
   <si>
     <t>Brief Description of Acomplishments</t>
   </si>
@@ -110,10 +110,6 @@
   </si>
   <si>
     <t>Researched/proposed development environments (IDEs) compatible with possible languages and frameworks to be used.</t>
-  </si>
-  <si>
-    <t>Sprint1.doc; 
-Sprint1.pptx</t>
   </si>
   <si>
     <t>Luis Ramirez</t>
@@ -135,9 +131,6 @@
   <si>
     <t>Designed/created sign up form for users,
 worked on information for Sprint 2 presentation(class diagram and Quality Assurance tests), and provided user stories.</t>
-  </si>
-  <si>
-    <t>1, 2, 3, 5, 6[CS,IT]</t>
   </si>
   <si>
     <t xml:space="preserve">https://github.com/quentinxs/GPTMS/tree/Luis/front-end/src/app
@@ -146,16 +139,43 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">front-end folder
-Sprint2.pptx
-User Stories.docx
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">signup folder
 Slides 3, 5-7
 Sprint 2 and 3 stories
 </t>
+  </si>
+  <si>
+    <t>1, 3, 5, 6[CS, IT]</t>
+  </si>
+  <si>
+    <t>1, 2, 3, 5, 6[CS, IT]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">front-end folder
+Sprint 2.pptx
+User Stories.docx
+</t>
+  </si>
+  <si>
+    <t>Sprint 1.doc; 
+Sprint 1.pptx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">front-end folder
+Sprint 3.pptx
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/quentinxs/GPTMS/tree/Luis/front-end/src/app
+https://github.com/quentinxs/GPTMS/blob/Luis/docs/presentations/Sprint%203.pptx
+</t>
+  </si>
+  <si>
+    <t>Continued to design/revise front end UI for users once they are logged in (navigation bar, edit profile, user landing page) and signup/login forms. Assisted with user stories and Sprint 3 presentation</t>
+  </si>
+  <si>
+    <t>signup folder, navbar folder, profile folder.
+Slides 2-3</t>
   </si>
 </sst>
 </file>
@@ -322,7 +342,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -365,6 +385,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -694,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -711,38 +734,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+    </row>
+    <row r="2" spans="1:8" ht="41.1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="21"/>
+      <c r="C2" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-    </row>
-    <row r="2" spans="1:8" ht="41.1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="26"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="22"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="4" t="s">
         <v>7</v>
       </c>
@@ -763,12 +786,12 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="114.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="23"/>
+      <c r="B4" s="24"/>
       <c r="C4" s="11">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>25</v>
@@ -777,56 +800,68 @@
         <v>26</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="G4" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="12" t="s">
+    </row>
+    <row r="5" spans="1:8" ht="165.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="24"/>
+      <c r="C5" s="14">
+        <v>18</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="165.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="14">
-        <v>16</v>
-      </c>
-      <c r="D5" s="15" t="s">
+      <c r="F5" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="16" t="s">
+    </row>
+    <row r="6" spans="1:8" ht="152.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="24"/>
+      <c r="C6" s="17">
+        <v>20</v>
+      </c>
+      <c r="D6" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="E6" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="17"/>
+      <c r="B7" s="18"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="2"/>
@@ -835,10 +870,10 @@
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="17"/>
+      <c r="B8" s="18"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="2"/>
@@ -847,10 +882,10 @@
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="17"/>
+      <c r="B9" s="18"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="2"/>
@@ -859,10 +894,10 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="17"/>
+      <c r="B10" s="18"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="2"/>
@@ -871,10 +906,10 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="17"/>
+      <c r="B11" s="18"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="2"/>
@@ -883,10 +918,10 @@
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="17"/>
+      <c r="B12" s="18"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="2"/>
@@ -895,10 +930,10 @@
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="17"/>
+      <c r="B13" s="18"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="2"/>
@@ -907,10 +942,10 @@
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="17"/>
+      <c r="B14" s="18"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="2"/>
@@ -919,10 +954,10 @@
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="17"/>
+      <c r="B15" s="18"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="2"/>
@@ -960,8 +995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -974,47 +1009,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="30" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+    </row>
+    <row r="2" spans="1:9" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="21"/>
+      <c r="C2" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-    </row>
-    <row r="2" spans="1:9" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="21"/>
     </row>
     <row r="3" spans="1:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="29" t="s">
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
     </row>
     <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -1050,7 +1085,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="8">
         <v>0</v>
@@ -1068,10 +1103,10 @@
         <v>0</v>
       </c>
       <c r="H5" s="8">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="I5" s="8">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -1079,7 +1114,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" s="8">
         <v>0</v>
@@ -1097,10 +1132,10 @@
         <v>0</v>
       </c>
       <c r="H6" s="8">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="I6" s="8">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
@@ -1108,42 +1143,58 @@
         <v>2</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" s="8">
+        <v>2</v>
+      </c>
+      <c r="D7" s="8">
+        <v>2</v>
+      </c>
+      <c r="E7" s="8">
+        <v>3</v>
+      </c>
+      <c r="F7" s="8">
+        <v>0</v>
+      </c>
+      <c r="G7" s="8">
+        <v>3</v>
+      </c>
+      <c r="H7" s="8">
+        <v>4</v>
+      </c>
+      <c r="I7" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>3</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="8">
         <v>1</v>
       </c>
-      <c r="D7" s="8">
-        <v>1</v>
-      </c>
-      <c r="E7" s="8">
-        <v>1</v>
-      </c>
-      <c r="F7" s="8">
-        <v>0</v>
-      </c>
-      <c r="G7" s="8">
+      <c r="D8" s="8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="8">
         <v>2</v>
       </c>
-      <c r="H7" s="8">
+      <c r="F8" s="8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="8">
         <v>3</v>
       </c>
-      <c r="I7" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
-        <v>3</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
+      <c r="H8" s="8">
+        <v>7</v>
+      </c>
+      <c r="I8" s="8">
+        <v>7</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
@@ -1220,5 +1271,6 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update effort log and sprint 4 pptx
</commit_message>
<xml_diff>
--- a/docs/efforts/Luis Ramirez.xlsx
+++ b/docs/efforts/Luis Ramirez.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LouieBoy\Documents\GitHub\GPTMS\docs\efforts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18F1920B-954C-4518-B65F-12AF62E3E5DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5EA0A79-1D46-4A6E-8C98-01D1F6E0A552}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11835" yWindow="1815" windowWidth="16935" windowHeight="11490" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15345" yWindow="225" windowWidth="13425" windowHeight="14145" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Evidence" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
   <si>
     <t>Brief Description of Acomplishments</t>
   </si>
@@ -176,6 +176,24 @@
   <si>
     <t>signup folder, navbar folder, profile folder.
 Slides 2-3</t>
+  </si>
+  <si>
+    <t>Worked on frontend development of user profile forms, scorecard design.
+Fixed navbar reponsiveness and routing.
+Helped with presentation powerpoint.</t>
+  </si>
+  <si>
+    <t>front-end folder
+Sprint 4.pptx</t>
+  </si>
+  <si>
+    <t>https://github.com/quentinxs/GPTMS/tree/Luis/front-end/src/app/navbar
+https://github.com/quentinxs/GPTMS/tree/Luis/front-end/src/app/profile
+https://github.com/quentinxs/GPTMS/blob/master/front-end/src/app/play/play.component.html</t>
+  </si>
+  <si>
+    <t>navbar folder, profile folder, play folder
+Slides 2 and 4</t>
   </si>
 </sst>
 </file>
@@ -342,7 +360,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -390,6 +408,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -410,18 +443,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -433,6 +454,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -717,8 +741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -734,38 +758,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
     </row>
     <row r="2" spans="1:8" ht="41.1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="19" t="s">
+      <c r="B2" s="26"/>
+      <c r="C2" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="27"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="21"/>
     </row>
     <row r="3" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="23"/>
+      <c r="B3" s="28"/>
       <c r="C3" s="4" t="s">
         <v>7</v>
       </c>
@@ -786,10 +810,10 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="114.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="24"/>
+      <c r="B4" s="29"/>
       <c r="C4" s="11">
         <v>17</v>
       </c>
@@ -810,10 +834,10 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="165.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="24"/>
+      <c r="B5" s="29"/>
       <c r="C5" s="14">
         <v>18</v>
       </c>
@@ -834,10 +858,10 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="152.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="24"/>
+      <c r="B6" s="29"/>
       <c r="C6" s="17">
         <v>20</v>
       </c>
@@ -857,23 +881,35 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+    <row r="7" spans="1:8" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="18">
+        <v>16</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="18"/>
+      <c r="B8" s="23"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="2"/>
@@ -882,10 +918,10 @@
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="18"/>
+      <c r="B9" s="23"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="2"/>
@@ -894,10 +930,10 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="18"/>
+      <c r="B10" s="23"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="2"/>
@@ -906,10 +942,10 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="18"/>
+      <c r="B11" s="23"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="2"/>
@@ -918,10 +954,10 @@
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="18"/>
+      <c r="B12" s="23"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="2"/>
@@ -930,10 +966,10 @@
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="18"/>
+      <c r="B13" s="23"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="2"/>
@@ -942,10 +978,10 @@
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="18"/>
+      <c r="B14" s="23"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="2"/>
@@ -954,10 +990,10 @@
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="18"/>
+      <c r="B15" s="23"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="2"/>
@@ -967,11 +1003,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="A2:B2"/>
@@ -985,6 +1016,11 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -996,7 +1032,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1009,47 +1045,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="31" t="s">
+      <c r="B1" s="33"/>
+      <c r="C1" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
     </row>
     <row r="2" spans="1:9" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="19" t="s">
+      <c r="B2" s="26"/>
+      <c r="C2" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="21"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="26"/>
     </row>
     <row r="3" spans="1:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="30" t="s">
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
     </row>
     <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -1197,17 +1233,33 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
+      <c r="A9" s="8">
         <v>4</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
+      <c r="B9" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="8">
+        <v>1</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0</v>
+      </c>
+      <c r="E9" s="8">
+        <v>2</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0</v>
+      </c>
+      <c r="G9" s="8">
+        <v>3</v>
+      </c>
+      <c r="H9" s="8">
+        <v>5</v>
+      </c>
+      <c r="I9" s="8">
+        <v>5</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7">

</xml_diff>